<commit_message>
MoeLotl Faction Expand 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/MoeLotl Faction Expand - 3412260468/3412260468.xlsx
+++ b/Data/MoeLotl Faction Expand - 3412260468/3412260468.xlsx
@@ -841,6 +841,30 @@
     <x:t>격세 가면이 사용자의 눈을 보호합니다</x:t>
   </x:si>
   <x:si>
+    <x:t>HediffDef+Axolotl_HealSelf.label</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Axolotl_HealSelf.label</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생명력 흡수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HediffDef+Axolotl_HealSelf.description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Axolotl_HealSelf.description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>시체의 생명력을 흡수하여 빠르게 상처를 회복합니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HediffDef+Axolotl_HealSelf.descriptionShort</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Axolotl_HealSelf.descriptionShort</x:t>
+  </x:si>
+  <x:si>
     <x:t>HistoryEventDef+Axolotl_CommunicateWithEvilSects.label</x:t>
   </x:si>
   <x:si>
@@ -853,6 +877,15 @@
     <x:t>사문과 결탁함</x:t>
   </x:si>
   <x:si>
+    <x:t>HistoryEventDef+Axolotl_UseCrimsonBloodPill.label</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Axolotl_UseCrimsonBloodPill.label</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사도에 들어섬</x:t>
+  </x:si>
+  <x:si>
     <x:t>HistoryEventDef+Axolotl_EnforceJusticeOnBehalfOfHeaven.label</x:t>
   </x:si>
   <x:si>
@@ -886,6 +919,15 @@
     <x:t>TargetA 채우는 중</x:t>
   </x:si>
   <x:si>
+    <x:t>JobDef+Axolotl_HealSelf.reportString</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Axolotl_HealSelf.reportString</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TargetA의 생명력 흡수 중</x:t>
+  </x:si>
+  <x:si>
     <x:t>MentalStateDef+Axolotl_ParasitismBerserk.label</x:t>
   </x:si>
   <x:si>
@@ -1384,7 +1426,7 @@
     <x:t>OminousLotlQiOverView_Energy_Tip</x:t>
   </x:si>
   <x:si>
-    <x:t>모에로틀 사수들이 개척한 새로운 수련 경로입니다.\n이 수련법은 자신의 생명을 끊임없이 착취해야만 완성할 수 있습니다.</x:t>
+    <x:t>모에로틀 사수들이 개척한 새로운 수련 경로입니다.\n이 수련법은 자신의 생명력을 끊임없이 착취해야만 완성할 수 있습니다.</x:t>
   </x:si>
   <x:si>
     <x:t>Keyed+OminousLotlQiOverView_Energy_Label</x:t>
@@ -1414,6 +1456,24 @@
     <x:t>식혈 보호막</x:t>
   </x:si>
   <x:si>
+    <x:t>Keyed+OminousLotlQiOverView_HealSelf_Tip</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OminousLotlQiOverView_HealSelf_Tip</x:t>
+  </x:si>
+  <x:si>
+    <x:t>시체의 생명력을 착취하여 자신의 생기를 보충합니다.\n이들이 사수라 불리는 이유는 자신의 생명력으로도 모자라 다른 사람의 생명력까지 착취하기 때문입니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Keyed+CompAxolotlOminousEnergy_HealSelf_MouseAttachedLabel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CompAxolotlOminousEnergy_HealSelf_MouseAttachedLabel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>시체 선택</x:t>
+  </x:si>
+  <x:si>
     <x:t>Keyed+Hediff_ConsciousnessOrgan_Tips</x:t>
   </x:si>
   <x:si>
@@ -1645,7 +1705,7 @@
     <x:t>Axolotl_MurderCeremonyBuilding_lastTime</x:t>
   </x:si>
   <x:si>
-    <x:t>경고： 의식 완료까지 {0}시간 남음</x:t>
+    <x:t>경고: 의식 완료까지 {0}시간 남음</x:t>
   </x:si>
   <x:si>
     <x:t>Keyed+Building_MurderCeremonyBuilding_String_NoStuff</x:t>
@@ -2088,7 +2148,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F194"/>
+  <x:dimension ref="A1:F201"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -3453,161 +3513,161 @@
         <x:v>275</x:v>
       </x:c>
       <x:c r="B97" s="1" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="C97" s="1" t="s">
         <x:v>276</x:v>
       </x:c>
-      <x:c r="C97" s="1" t="s">
+      <x:c r="F97" s="1" t="s">
         <x:v>277</x:v>
-      </x:c>
-      <x:c r="F97" s="1" t="s">
-        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:6">
       <x:c r="A98" s="1" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="B98" s="1" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="C98" s="1" t="s">
         <x:v>279</x:v>
       </x:c>
-      <x:c r="B98" s="1" t="s">
-        <x:v>276</x:v>
-      </x:c>
-      <x:c r="C98" s="1" t="s">
+      <x:c r="F98" s="1" t="s">
         <x:v>280</x:v>
-      </x:c>
-      <x:c r="F98" s="1" t="s">
-        <x:v>281</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:6">
       <x:c r="A99" s="1" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="B99" s="1" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="C99" s="1" t="s">
         <x:v>282</x:v>
       </x:c>
-      <x:c r="B99" s="1" t="s">
-        <x:v>283</x:v>
-      </x:c>
-      <x:c r="C99" s="1" t="s">
-        <x:v>284</x:v>
-      </x:c>
       <x:c r="F99" s="1" t="s">
-        <x:v>285</x:v>
+        <x:v>280</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:6">
       <x:c r="A100" s="1" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="B100" s="1" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="C100" s="1" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="F100" s="1" t="s">
         <x:v>286</x:v>
-      </x:c>
-      <x:c r="B100" s="1" t="s">
-        <x:v>287</x:v>
-      </x:c>
-      <x:c r="C100" s="1" t="s">
-        <x:v>288</x:v>
-      </x:c>
-      <x:c r="F100" s="1" t="s">
-        <x:v>289</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:6">
       <x:c r="A101" s="1" t="s">
-        <x:v>290</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="B101" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="C101" s="1" t="s">
-        <x:v>292</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="F101" s="1" t="s">
-        <x:v>293</x:v>
+        <x:v>289</x:v>
       </x:c>
     </x:row>
     <x:row r="102" spans="1:6">
       <x:c r="A102" s="1" t="s">
-        <x:v>294</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B102" s="1" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="C102" s="1" t="s">
         <x:v>291</x:v>
       </x:c>
-      <x:c r="C102" s="1" t="s">
-        <x:v>295</x:v>
-      </x:c>
       <x:c r="F102" s="1" t="s">
-        <x:v>296</x:v>
+        <x:v>292</x:v>
       </x:c>
     </x:row>
     <x:row r="103" spans="1:6">
       <x:c r="A103" s="1" t="s">
-        <x:v>297</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="B103" s="1" t="s">
-        <x:v>298</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="C103" s="1" t="s">
-        <x:v>299</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="F103" s="1" t="s">
-        <x:v>300</x:v>
+        <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="104" spans="1:6">
       <x:c r="A104" s="1" t="s">
-        <x:v>301</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="B104" s="1" t="s">
         <x:v>298</x:v>
       </x:c>
       <x:c r="C104" s="1" t="s">
-        <x:v>302</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="F104" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:6">
       <x:c r="A105" s="1" t="s">
-        <x:v>303</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="B105" s="1" t="s">
         <x:v>298</x:v>
       </x:c>
       <x:c r="C105" s="1" t="s">
-        <x:v>304</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="F105" s="1" t="s">
-        <x:v>305</x:v>
+        <x:v>303</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:6">
       <x:c r="A106" s="1" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="B106" s="1" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="C106" s="1" t="s">
         <x:v>306</x:v>
       </x:c>
-      <x:c r="B106" s="1" t="s">
-        <x:v>298</x:v>
-      </x:c>
-      <x:c r="C106" s="1" t="s">
+      <x:c r="F106" s="1" t="s">
         <x:v>307</x:v>
-      </x:c>
-      <x:c r="F106" s="1" t="s">
-        <x:v>308</x:v>
       </x:c>
     </x:row>
     <x:row r="107" spans="1:6">
       <x:c r="A107" s="1" t="s">
+        <x:v>308</x:v>
+      </x:c>
+      <x:c r="B107" s="1" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="C107" s="1" t="s">
         <x:v>309</x:v>
       </x:c>
-      <x:c r="B107" s="1" t="s">
-        <x:v>298</x:v>
-      </x:c>
-      <x:c r="C107" s="1" t="s">
+      <x:c r="F107" s="1" t="s">
         <x:v>310</x:v>
-      </x:c>
-      <x:c r="F107" s="1" t="s">
-        <x:v>311</x:v>
       </x:c>
     </x:row>
     <x:row r="108" spans="1:6">
       <x:c r="A108" s="1" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="B108" s="1" t="s">
         <x:v>312</x:v>
-      </x:c>
-      <x:c r="B108" s="1" t="s">
-        <x:v>298</x:v>
       </x:c>
       <x:c r="C108" s="1" t="s">
         <x:v>313</x:v>
@@ -3621,164 +3681,164 @@
         <x:v>315</x:v>
       </x:c>
       <x:c r="B109" s="1" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="C109" s="1" t="s">
         <x:v>316</x:v>
       </x:c>
-      <x:c r="C109" s="1" t="s">
-        <x:v>317</x:v>
-      </x:c>
       <x:c r="F109" s="1" t="s">
-        <x:v>318</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:6">
       <x:c r="A110" s="1" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="B110" s="1" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="C110" s="1" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="F110" s="1" t="s">
         <x:v>319</x:v>
-      </x:c>
-      <x:c r="B110" s="1" t="s">
-        <x:v>316</x:v>
-      </x:c>
-      <x:c r="C110" s="1" t="s">
-        <x:v>320</x:v>
-      </x:c>
-      <x:c r="F110" s="1" t="s">
-        <x:v>321</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:6">
       <x:c r="A111" s="1" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="B111" s="1" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="C111" s="1" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="F111" s="1" t="s">
         <x:v>322</x:v>
-      </x:c>
-      <x:c r="B111" s="1" t="s">
-        <x:v>323</x:v>
-      </x:c>
-      <x:c r="C111" s="1" t="s">
-        <x:v>324</x:v>
-      </x:c>
-      <x:c r="F111" s="1" t="s">
-        <x:v>325</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:6">
       <x:c r="A112" s="1" t="s">
-        <x:v>326</x:v>
+        <x:v>323</x:v>
       </x:c>
       <x:c r="B112" s="1" t="s">
-        <x:v>323</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="C112" s="1" t="s">
-        <x:v>327</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="F112" s="1" t="s">
-        <x:v>328</x:v>
+        <x:v>325</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:6">
       <x:c r="A113" s="1" t="s">
-        <x:v>329</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="B113" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="C113" s="1" t="s">
-        <x:v>331</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="F113" s="1" t="s">
-        <x:v>332</x:v>
+        <x:v>328</x:v>
       </x:c>
     </x:row>
     <x:row r="114" spans="1:6">
       <x:c r="A114" s="1" t="s">
-        <x:v>333</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="B114" s="1" t="s">
         <x:v>330</x:v>
       </x:c>
       <x:c r="C114" s="1" t="s">
-        <x:v>334</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="F114" s="1" t="s">
-        <x:v>335</x:v>
+        <x:v>332</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:6">
       <x:c r="A115" s="1" t="s">
-        <x:v>336</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="B115" s="1" t="s">
         <x:v>330</x:v>
       </x:c>
       <x:c r="C115" s="1" t="s">
-        <x:v>337</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="F115" s="1" t="s">
-        <x:v>338</x:v>
+        <x:v>335</x:v>
       </x:c>
     </x:row>
     <x:row r="116" spans="1:6">
       <x:c r="A116" s="1" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="B116" s="1" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C116" s="1" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="F116" s="1" t="s">
         <x:v>339</x:v>
-      </x:c>
-      <x:c r="B116" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C116" s="1" t="s">
-        <x:v>340</x:v>
-      </x:c>
-      <x:c r="F116" s="1" t="s">
-        <x:v>341</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:6">
       <x:c r="A117" s="1" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="B117" s="1" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C117" s="1" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="F117" s="1" t="s">
         <x:v>342</x:v>
-      </x:c>
-      <x:c r="B117" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C117" s="1" t="s">
-        <x:v>343</x:v>
-      </x:c>
-      <x:c r="F117" s="1" t="s">
-        <x:v>344</x:v>
       </x:c>
     </x:row>
     <x:row r="118" spans="1:6">
       <x:c r="A118" s="1" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="B118" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C118" s="1" t="s">
         <x:v>345</x:v>
       </x:c>
-      <x:c r="B118" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C118" s="1" t="s">
+      <x:c r="F118" s="1" t="s">
         <x:v>346</x:v>
-      </x:c>
-      <x:c r="F118" s="1" t="s">
-        <x:v>347</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:6">
       <x:c r="A119" s="1" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="B119" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C119" s="1" t="s">
         <x:v>348</x:v>
       </x:c>
-      <x:c r="B119" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C119" s="1" t="s">
+      <x:c r="F119" s="1" t="s">
         <x:v>349</x:v>
-      </x:c>
-      <x:c r="F119" s="1" t="s">
-        <x:v>350</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:6">
       <x:c r="A120" s="1" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="B120" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C120" s="1" t="s">
         <x:v>351</x:v>
-      </x:c>
-      <x:c r="B120" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C120" s="1" t="s">
-        <x:v>267</x:v>
       </x:c>
       <x:c r="F120" s="1" t="s">
         <x:v>352</x:v>
@@ -3789,80 +3849,80 @@
         <x:v>353</x:v>
       </x:c>
       <x:c r="B121" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C121" s="1" t="s">
-        <x:v>270</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="F121" s="1" t="s">
-        <x:v>354</x:v>
+        <x:v>355</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:6">
       <x:c r="A122" s="1" t="s">
-        <x:v>355</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="B122" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C122" s="1" t="s">
-        <x:v>356</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="F122" s="1" t="s">
-        <x:v>357</x:v>
+        <x:v>358</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:6">
       <x:c r="A123" s="1" t="s">
-        <x:v>358</x:v>
+        <x:v>359</x:v>
       </x:c>
       <x:c r="B123" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C123" s="1" t="s">
-        <x:v>359</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="F123" s="1" t="s">
-        <x:v>360</x:v>
+        <x:v>361</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:6">
       <x:c r="A124" s="1" t="s">
-        <x:v>361</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="B124" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C124" s="1" t="s">
-        <x:v>362</x:v>
+        <x:v>363</x:v>
       </x:c>
       <x:c r="F124" s="1" t="s">
-        <x:v>244</x:v>
+        <x:v>364</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:6">
       <x:c r="A125" s="1" t="s">
-        <x:v>363</x:v>
+        <x:v>365</x:v>
       </x:c>
       <x:c r="B125" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C125" s="1" t="s">
-        <x:v>364</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F125" s="1" t="s">
-        <x:v>365</x:v>
+        <x:v>366</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:6">
       <x:c r="A126" s="1" t="s">
-        <x:v>366</x:v>
+        <x:v>367</x:v>
       </x:c>
       <x:c r="B126" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C126" s="1" t="s">
-        <x:v>367</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="F126" s="1" t="s">
         <x:v>368</x:v>
@@ -3873,83 +3933,83 @@
         <x:v>369</x:v>
       </x:c>
       <x:c r="B127" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C127" s="1" t="s">
         <x:v>370</x:v>
       </x:c>
       <x:c r="F127" s="1" t="s">
-        <x:v>260</x:v>
+        <x:v>371</x:v>
       </x:c>
     </x:row>
     <x:row r="128" spans="1:6">
       <x:c r="A128" s="1" t="s">
-        <x:v>371</x:v>
+        <x:v>372</x:v>
       </x:c>
       <x:c r="B128" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C128" s="1" t="s">
-        <x:v>372</x:v>
+        <x:v>373</x:v>
       </x:c>
       <x:c r="F128" s="1" t="s">
-        <x:v>373</x:v>
+        <x:v>374</x:v>
       </x:c>
     </x:row>
     <x:row r="129" spans="1:6">
       <x:c r="A129" s="1" t="s">
-        <x:v>374</x:v>
+        <x:v>375</x:v>
       </x:c>
       <x:c r="B129" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C129" s="1" t="s">
-        <x:v>375</x:v>
+        <x:v>376</x:v>
       </x:c>
       <x:c r="F129" s="1" t="s">
-        <x:v>368</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:6">
       <x:c r="A130" s="1" t="s">
-        <x:v>376</x:v>
+        <x:v>377</x:v>
       </x:c>
       <x:c r="B130" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C130" s="1" t="s">
-        <x:v>377</x:v>
+        <x:v>378</x:v>
       </x:c>
       <x:c r="F130" s="1" t="s">
-        <x:v>378</x:v>
+        <x:v>379</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:6">
       <x:c r="A131" s="1" t="s">
-        <x:v>379</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="B131" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C131" s="1" t="s">
-        <x:v>380</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="F131" s="1" t="s">
-        <x:v>381</x:v>
+        <x:v>382</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:6">
       <x:c r="A132" s="1" t="s">
-        <x:v>382</x:v>
+        <x:v>383</x:v>
       </x:c>
       <x:c r="B132" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C132" s="1" t="s">
-        <x:v>383</x:v>
+        <x:v>384</x:v>
       </x:c>
       <x:c r="F132" s="1" t="s">
-        <x:v>384</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:6">
@@ -3957,7 +4017,7 @@
         <x:v>385</x:v>
       </x:c>
       <x:c r="B133" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C133" s="1" t="s">
         <x:v>386</x:v>
@@ -3971,125 +4031,125 @@
         <x:v>388</x:v>
       </x:c>
       <x:c r="B134" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C134" s="1" t="s">
         <x:v>389</x:v>
       </x:c>
       <x:c r="F134" s="1" t="s">
-        <x:v>390</x:v>
+        <x:v>382</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:6">
       <x:c r="A135" s="1" t="s">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="B135" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C135" s="1" t="s">
         <x:v>391</x:v>
       </x:c>
-      <x:c r="B135" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C135" s="1" t="s">
+      <x:c r="F135" s="1" t="s">
         <x:v>392</x:v>
-      </x:c>
-      <x:c r="F135" s="1" t="s">
-        <x:v>393</x:v>
       </x:c>
     </x:row>
     <x:row r="136" spans="1:6">
       <x:c r="A136" s="1" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="B136" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C136" s="1" t="s">
         <x:v>394</x:v>
       </x:c>
-      <x:c r="B136" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C136" s="1" t="s">
+      <x:c r="F136" s="1" t="s">
         <x:v>395</x:v>
-      </x:c>
-      <x:c r="F136" s="1" t="s">
-        <x:v>396</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:6">
       <x:c r="A137" s="1" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="B137" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C137" s="1" t="s">
         <x:v>397</x:v>
       </x:c>
-      <x:c r="B137" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C137" s="1" t="s">
+      <x:c r="F137" s="1" t="s">
         <x:v>398</x:v>
-      </x:c>
-      <x:c r="F137" s="1" t="s">
-        <x:v>399</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:6">
       <x:c r="A138" s="1" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="B138" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C138" s="1" t="s">
         <x:v>400</x:v>
       </x:c>
-      <x:c r="B138" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C138" s="1" t="s">
+      <x:c r="F138" s="1" t="s">
         <x:v>401</x:v>
-      </x:c>
-      <x:c r="F138" s="1" t="s">
-        <x:v>402</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:6">
       <x:c r="A139" s="1" t="s">
+        <x:v>402</x:v>
+      </x:c>
+      <x:c r="B139" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C139" s="1" t="s">
         <x:v>403</x:v>
       </x:c>
-      <x:c r="B139" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C139" s="1" t="s">
+      <x:c r="F139" s="1" t="s">
         <x:v>404</x:v>
-      </x:c>
-      <x:c r="F139" s="1" t="s">
-        <x:v>405</x:v>
       </x:c>
     </x:row>
     <x:row r="140" spans="1:6">
       <x:c r="A140" s="1" t="s">
+        <x:v>405</x:v>
+      </x:c>
+      <x:c r="B140" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C140" s="1" t="s">
         <x:v>406</x:v>
       </x:c>
-      <x:c r="B140" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C140" s="1" t="s">
+      <x:c r="F140" s="1" t="s">
         <x:v>407</x:v>
-      </x:c>
-      <x:c r="F140" s="1" t="s">
-        <x:v>408</x:v>
       </x:c>
     </x:row>
     <x:row r="141" spans="1:6">
       <x:c r="A141" s="1" t="s">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="B141" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C141" s="1" t="s">
         <x:v>409</x:v>
       </x:c>
-      <x:c r="B141" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C141" s="1" t="s">
+      <x:c r="F141" s="1" t="s">
         <x:v>410</x:v>
-      </x:c>
-      <x:c r="F141" s="1" t="s">
-        <x:v>411</x:v>
       </x:c>
     </x:row>
     <x:row r="142" spans="1:6">
       <x:c r="A142" s="1" t="s">
+        <x:v>411</x:v>
+      </x:c>
+      <x:c r="B142" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C142" s="1" t="s">
         <x:v>412</x:v>
       </x:c>
-      <x:c r="B142" s="1" t="s">
-        <x:v>330</x:v>
-      </x:c>
-      <x:c r="C142" s="1" t="s">
+      <x:c r="F142" s="1" t="s">
         <x:v>413</x:v>
-      </x:c>
-      <x:c r="F142" s="1" t="s">
-        <x:v>399</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:6">
@@ -4097,69 +4157,69 @@
         <x:v>414</x:v>
       </x:c>
       <x:c r="B143" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C143" s="1" t="s">
         <x:v>415</x:v>
       </x:c>
       <x:c r="F143" s="1" t="s">
-        <x:v>402</x:v>
+        <x:v>416</x:v>
       </x:c>
     </x:row>
     <x:row r="144" spans="1:6">
       <x:c r="A144" s="1" t="s">
-        <x:v>416</x:v>
+        <x:v>417</x:v>
       </x:c>
       <x:c r="B144" s="1" t="s">
-        <x:v>330</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C144" s="1" t="s">
-        <x:v>417</x:v>
+        <x:v>418</x:v>
       </x:c>
       <x:c r="F144" s="1" t="s">
-        <x:v>405</x:v>
+        <x:v>419</x:v>
       </x:c>
     </x:row>
     <x:row r="145" spans="1:6">
       <x:c r="A145" s="1" t="s">
-        <x:v>418</x:v>
+        <x:v>420</x:v>
       </x:c>
       <x:c r="B145" s="1" t="s">
-        <x:v>419</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C145" s="1" t="s">
-        <x:v>420</x:v>
+        <x:v>421</x:v>
       </x:c>
       <x:c r="F145" s="1" t="s">
-        <x:v>421</x:v>
+        <x:v>422</x:v>
       </x:c>
     </x:row>
     <x:row r="146" spans="1:6">
       <x:c r="A146" s="1" t="s">
-        <x:v>422</x:v>
+        <x:v>423</x:v>
       </x:c>
       <x:c r="B146" s="1" t="s">
-        <x:v>419</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C146" s="1" t="s">
-        <x:v>423</x:v>
+        <x:v>424</x:v>
       </x:c>
       <x:c r="F146" s="1" t="s">
-        <x:v>424</x:v>
+        <x:v>425</x:v>
       </x:c>
     </x:row>
     <x:row r="147" spans="1:6">
       <x:c r="A147" s="1" t="s">
-        <x:v>425</x:v>
+        <x:v>426</x:v>
       </x:c>
       <x:c r="B147" s="1" t="s">
-        <x:v>419</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C147" s="1" t="s">
-        <x:v>426</x:v>
+        <x:v>427</x:v>
       </x:c>
       <x:c r="F147" s="1" t="s">
-        <x:v>427</x:v>
+        <x:v>413</x:v>
       </x:c>
     </x:row>
     <x:row r="148" spans="1:6">
@@ -4167,559 +4227,559 @@
         <x:v>428</x:v>
       </x:c>
       <x:c r="B148" s="1" t="s">
-        <x:v>419</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="C148" s="1" t="s">
         <x:v>429</x:v>
       </x:c>
       <x:c r="F148" s="1" t="s">
-        <x:v>430</x:v>
+        <x:v>416</x:v>
       </x:c>
     </x:row>
     <x:row r="149" spans="1:6">
       <x:c r="A149" s="1" t="s">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="B149" s="1" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="C149" s="1" t="s">
         <x:v>431</x:v>
       </x:c>
-      <x:c r="B149" s="1" t="s">
+      <x:c r="F149" s="1" t="s">
         <x:v>419</x:v>
-      </x:c>
-      <x:c r="C149" s="1" t="s">
-        <x:v>432</x:v>
-      </x:c>
-      <x:c r="F149" s="1" t="s">
-        <x:v>433</x:v>
       </x:c>
     </x:row>
     <x:row r="150" spans="1:6">
       <x:c r="A150" s="1" t="s">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c r="B150" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C150" s="1" t="s">
         <x:v>434</x:v>
       </x:c>
-      <x:c r="B150" s="1" t="s">
-        <x:v>419</x:v>
-      </x:c>
-      <x:c r="C150" s="1" t="s">
+      <x:c r="F150" s="1" t="s">
         <x:v>435</x:v>
-      </x:c>
-      <x:c r="F150" s="1" t="s">
-        <x:v>436</x:v>
       </x:c>
     </x:row>
     <x:row r="151" spans="1:6">
       <x:c r="A151" s="1" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="B151" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C151" s="1" t="s">
         <x:v>437</x:v>
       </x:c>
-      <x:c r="B151" s="1" t="s">
-        <x:v>419</x:v>
-      </x:c>
-      <x:c r="C151" s="1" t="s">
+      <x:c r="F151" s="1" t="s">
         <x:v>438</x:v>
-      </x:c>
-      <x:c r="F151" s="1" t="s">
-        <x:v>439</x:v>
       </x:c>
     </x:row>
     <x:row r="152" spans="1:6">
       <x:c r="A152" s="1" t="s">
+        <x:v>439</x:v>
+      </x:c>
+      <x:c r="B152" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C152" s="1" t="s">
         <x:v>440</x:v>
       </x:c>
-      <x:c r="B152" s="1" t="s">
-        <x:v>419</x:v>
-      </x:c>
-      <x:c r="C152" s="1" t="s">
+      <x:c r="F152" s="1" t="s">
         <x:v>441</x:v>
-      </x:c>
-      <x:c r="F152" s="1" t="s">
-        <x:v>442</x:v>
       </x:c>
     </x:row>
     <x:row r="153" spans="1:6">
       <x:c r="A153" s="1" t="s">
+        <x:v>442</x:v>
+      </x:c>
+      <x:c r="B153" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C153" s="1" t="s">
         <x:v>443</x:v>
       </x:c>
-      <x:c r="B153" s="1" t="s">
+      <x:c r="F153" s="1" t="s">
         <x:v>444</x:v>
-      </x:c>
-      <x:c r="C153" s="1" t="s">
-        <x:v>445</x:v>
-      </x:c>
-      <x:c r="F153" s="1" t="s">
-        <x:v>446</x:v>
       </x:c>
     </x:row>
     <x:row r="154" spans="1:6">
       <x:c r="A154" s="1" t="s">
+        <x:v>445</x:v>
+      </x:c>
+      <x:c r="B154" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C154" s="1" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="F154" s="1" t="s">
         <x:v>447</x:v>
-      </x:c>
-      <x:c r="B154" s="1" t="s">
-        <x:v>444</x:v>
-      </x:c>
-      <x:c r="C154" s="1" t="s">
-        <x:v>448</x:v>
-      </x:c>
-      <x:c r="F154" s="1" t="s">
-        <x:v>449</x:v>
       </x:c>
     </x:row>
     <x:row r="155" spans="1:6">
       <x:c r="A155" s="1" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="B155" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C155" s="1" t="s">
+        <x:v>449</x:v>
+      </x:c>
+      <x:c r="F155" s="1" t="s">
         <x:v>450</x:v>
-      </x:c>
-      <x:c r="B155" s="1" t="s">
-        <x:v>444</x:v>
-      </x:c>
-      <x:c r="C155" s="1" t="s">
-        <x:v>451</x:v>
-      </x:c>
-      <x:c r="F155" s="1" t="s">
-        <x:v>452</x:v>
       </x:c>
     </x:row>
     <x:row r="156" spans="1:6">
       <x:c r="A156" s="1" t="s">
+        <x:v>451</x:v>
+      </x:c>
+      <x:c r="B156" s="1" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="C156" s="1" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="F156" s="1" t="s">
         <x:v>453</x:v>
-      </x:c>
-      <x:c r="B156" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C156" s="1" t="s">
-        <x:v>455</x:v>
-      </x:c>
-      <x:c r="F156" s="1" t="s">
-        <x:v>456</x:v>
       </x:c>
     </x:row>
     <x:row r="157" spans="1:6">
       <x:c r="A157" s="1" t="s">
-        <x:v>457</x:v>
+        <x:v>454</x:v>
       </x:c>
       <x:c r="B157" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>433</x:v>
       </x:c>
       <x:c r="C157" s="1" t="s">
-        <x:v>458</x:v>
+        <x:v>455</x:v>
       </x:c>
       <x:c r="F157" s="1" t="s">
-        <x:v>459</x:v>
+        <x:v>456</x:v>
       </x:c>
     </x:row>
     <x:row r="158" spans="1:6">
       <x:c r="A158" s="1" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="B158" s="1" t="s">
+        <x:v>458</x:v>
+      </x:c>
+      <x:c r="C158" s="1" t="s">
+        <x:v>459</x:v>
+      </x:c>
+      <x:c r="F158" s="1" t="s">
         <x:v>460</x:v>
-      </x:c>
-      <x:c r="B158" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C158" s="1" t="s">
-        <x:v>461</x:v>
-      </x:c>
-      <x:c r="F158" s="1" t="s">
-        <x:v>462</x:v>
       </x:c>
     </x:row>
     <x:row r="159" spans="1:6">
       <x:c r="A159" s="1" t="s">
+        <x:v>461</x:v>
+      </x:c>
+      <x:c r="B159" s="1" t="s">
+        <x:v>458</x:v>
+      </x:c>
+      <x:c r="C159" s="1" t="s">
+        <x:v>462</x:v>
+      </x:c>
+      <x:c r="F159" s="1" t="s">
         <x:v>463</x:v>
-      </x:c>
-      <x:c r="B159" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C159" s="1" t="s">
-        <x:v>464</x:v>
-      </x:c>
-      <x:c r="F159" s="1" t="s">
-        <x:v>465</x:v>
       </x:c>
     </x:row>
     <x:row r="160" spans="1:6">
       <x:c r="A160" s="1" t="s">
+        <x:v>464</x:v>
+      </x:c>
+      <x:c r="B160" s="1" t="s">
+        <x:v>458</x:v>
+      </x:c>
+      <x:c r="C160" s="1" t="s">
+        <x:v>465</x:v>
+      </x:c>
+      <x:c r="F160" s="1" t="s">
         <x:v>466</x:v>
-      </x:c>
-      <x:c r="B160" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C160" s="1" t="s">
-        <x:v>467</x:v>
-      </x:c>
-      <x:c r="F160" s="1" t="s">
-        <x:v>468</x:v>
       </x:c>
     </x:row>
     <x:row r="161" spans="1:6">
       <x:c r="A161" s="1" t="s">
+        <x:v>467</x:v>
+      </x:c>
+      <x:c r="B161" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C161" s="1" t="s">
         <x:v>469</x:v>
       </x:c>
-      <x:c r="B161" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C161" s="1" t="s">
+      <x:c r="F161" s="1" t="s">
         <x:v>470</x:v>
-      </x:c>
-      <x:c r="F161" s="1" t="s">
-        <x:v>471</x:v>
       </x:c>
     </x:row>
     <x:row r="162" spans="1:6">
       <x:c r="A162" s="1" t="s">
+        <x:v>471</x:v>
+      </x:c>
+      <x:c r="B162" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C162" s="1" t="s">
         <x:v>472</x:v>
       </x:c>
-      <x:c r="B162" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C162" s="1" t="s">
+      <x:c r="F162" s="1" t="s">
         <x:v>473</x:v>
-      </x:c>
-      <x:c r="F162" s="1" t="s">
-        <x:v>474</x:v>
       </x:c>
     </x:row>
     <x:row r="163" spans="1:6">
       <x:c r="A163" s="1" t="s">
+        <x:v>474</x:v>
+      </x:c>
+      <x:c r="B163" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C163" s="1" t="s">
         <x:v>475</x:v>
       </x:c>
-      <x:c r="B163" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C163" s="1" t="s">
+      <x:c r="F163" s="1" t="s">
         <x:v>476</x:v>
-      </x:c>
-      <x:c r="F163" s="1" t="s">
-        <x:v>477</x:v>
       </x:c>
     </x:row>
     <x:row r="164" spans="1:6">
       <x:c r="A164" s="1" t="s">
+        <x:v>477</x:v>
+      </x:c>
+      <x:c r="B164" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C164" s="1" t="s">
         <x:v>478</x:v>
       </x:c>
-      <x:c r="B164" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C164" s="1" t="s">
+      <x:c r="F164" s="1" t="s">
         <x:v>479</x:v>
-      </x:c>
-      <x:c r="F164" s="1" t="s">
-        <x:v>480</x:v>
       </x:c>
     </x:row>
     <x:row r="165" spans="1:6">
       <x:c r="A165" s="1" t="s">
+        <x:v>480</x:v>
+      </x:c>
+      <x:c r="B165" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C165" s="1" t="s">
         <x:v>481</x:v>
       </x:c>
-      <x:c r="B165" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C165" s="1" t="s">
+      <x:c r="F165" s="1" t="s">
         <x:v>482</x:v>
-      </x:c>
-      <x:c r="F165" s="1" t="s">
-        <x:v>483</x:v>
       </x:c>
     </x:row>
     <x:row r="166" spans="1:6">
       <x:c r="A166" s="1" t="s">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="B166" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C166" s="1" t="s">
         <x:v>484</x:v>
       </x:c>
-      <x:c r="B166" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C166" s="1" t="s">
+      <x:c r="F166" s="1" t="s">
         <x:v>485</x:v>
-      </x:c>
-      <x:c r="F166" s="1" t="s">
-        <x:v>486</x:v>
       </x:c>
     </x:row>
     <x:row r="167" spans="1:6">
       <x:c r="A167" s="1" t="s">
+        <x:v>486</x:v>
+      </x:c>
+      <x:c r="B167" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C167" s="1" t="s">
         <x:v>487</x:v>
       </x:c>
-      <x:c r="B167" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C167" s="1" t="s">
+      <x:c r="F167" s="1" t="s">
         <x:v>488</x:v>
-      </x:c>
-      <x:c r="F167" s="1" t="s">
-        <x:v>489</x:v>
       </x:c>
     </x:row>
     <x:row r="168" spans="1:6">
       <x:c r="A168" s="1" t="s">
+        <x:v>489</x:v>
+      </x:c>
+      <x:c r="B168" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C168" s="1" t="s">
         <x:v>490</x:v>
       </x:c>
-      <x:c r="B168" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C168" s="1" t="s">
+      <x:c r="F168" s="1" t="s">
         <x:v>491</x:v>
-      </x:c>
-      <x:c r="F168" s="1" t="s">
-        <x:v>492</x:v>
       </x:c>
     </x:row>
     <x:row r="169" spans="1:6">
       <x:c r="A169" s="1" t="s">
+        <x:v>492</x:v>
+      </x:c>
+      <x:c r="B169" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C169" s="1" t="s">
         <x:v>493</x:v>
       </x:c>
-      <x:c r="B169" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C169" s="1" t="s">
+      <x:c r="F169" s="1" t="s">
         <x:v>494</x:v>
-      </x:c>
-      <x:c r="F169" s="1" t="s">
-        <x:v>495</x:v>
       </x:c>
     </x:row>
     <x:row r="170" spans="1:6">
       <x:c r="A170" s="1" t="s">
+        <x:v>495</x:v>
+      </x:c>
+      <x:c r="B170" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C170" s="1" t="s">
         <x:v>496</x:v>
       </x:c>
-      <x:c r="B170" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C170" s="1" t="s">
+      <x:c r="F170" s="1" t="s">
         <x:v>497</x:v>
-      </x:c>
-      <x:c r="F170" s="1" t="s">
-        <x:v>498</x:v>
       </x:c>
     </x:row>
     <x:row r="171" spans="1:6">
       <x:c r="A171" s="1" t="s">
+        <x:v>498</x:v>
+      </x:c>
+      <x:c r="B171" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C171" s="1" t="s">
         <x:v>499</x:v>
       </x:c>
-      <x:c r="B171" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C171" s="1" t="s">
+      <x:c r="F171" s="1" t="s">
         <x:v>500</x:v>
-      </x:c>
-      <x:c r="F171" s="1" t="s">
-        <x:v>501</x:v>
       </x:c>
     </x:row>
     <x:row r="172" spans="1:6">
       <x:c r="A172" s="1" t="s">
+        <x:v>501</x:v>
+      </x:c>
+      <x:c r="B172" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C172" s="1" t="s">
         <x:v>502</x:v>
       </x:c>
-      <x:c r="B172" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C172" s="1" t="s">
+      <x:c r="F172" s="1" t="s">
         <x:v>503</x:v>
-      </x:c>
-      <x:c r="F172" s="1" t="s">
-        <x:v>504</x:v>
       </x:c>
     </x:row>
     <x:row r="173" spans="1:6">
       <x:c r="A173" s="1" t="s">
+        <x:v>504</x:v>
+      </x:c>
+      <x:c r="B173" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C173" s="1" t="s">
         <x:v>505</x:v>
       </x:c>
-      <x:c r="B173" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C173" s="1" t="s">
+      <x:c r="F173" s="1" t="s">
         <x:v>506</x:v>
-      </x:c>
-      <x:c r="F173" s="1" t="s">
-        <x:v>507</x:v>
       </x:c>
     </x:row>
     <x:row r="174" spans="1:6">
       <x:c r="A174" s="1" t="s">
+        <x:v>507</x:v>
+      </x:c>
+      <x:c r="B174" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C174" s="1" t="s">
         <x:v>508</x:v>
       </x:c>
-      <x:c r="B174" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C174" s="1" t="s">
+      <x:c r="F174" s="1" t="s">
         <x:v>509</x:v>
-      </x:c>
-      <x:c r="F174" s="1" t="s">
-        <x:v>510</x:v>
       </x:c>
     </x:row>
     <x:row r="175" spans="1:6">
       <x:c r="A175" s="1" t="s">
+        <x:v>510</x:v>
+      </x:c>
+      <x:c r="B175" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C175" s="1" t="s">
         <x:v>511</x:v>
       </x:c>
-      <x:c r="B175" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C175" s="1" t="s">
+      <x:c r="F175" s="1" t="s">
         <x:v>512</x:v>
-      </x:c>
-      <x:c r="F175" s="1" t="s">
-        <x:v>513</x:v>
       </x:c>
     </x:row>
     <x:row r="176" spans="1:6">
       <x:c r="A176" s="1" t="s">
+        <x:v>513</x:v>
+      </x:c>
+      <x:c r="B176" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C176" s="1" t="s">
         <x:v>514</x:v>
       </x:c>
-      <x:c r="B176" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C176" s="1" t="s">
+      <x:c r="F176" s="1" t="s">
         <x:v>515</x:v>
-      </x:c>
-      <x:c r="F176" s="1" t="s">
-        <x:v>516</x:v>
       </x:c>
     </x:row>
     <x:row r="177" spans="1:6">
       <x:c r="A177" s="1" t="s">
+        <x:v>516</x:v>
+      </x:c>
+      <x:c r="B177" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C177" s="1" t="s">
         <x:v>517</x:v>
       </x:c>
-      <x:c r="B177" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C177" s="1" t="s">
+      <x:c r="F177" s="1" t="s">
         <x:v>518</x:v>
-      </x:c>
-      <x:c r="F177" s="1" t="s">
-        <x:v>519</x:v>
       </x:c>
     </x:row>
     <x:row r="178" spans="1:6">
       <x:c r="A178" s="1" t="s">
+        <x:v>519</x:v>
+      </x:c>
+      <x:c r="B178" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C178" s="1" t="s">
         <x:v>520</x:v>
       </x:c>
-      <x:c r="B178" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C178" s="1" t="s">
+      <x:c r="F178" s="1" t="s">
         <x:v>521</x:v>
-      </x:c>
-      <x:c r="F178" s="1" t="s">
-        <x:v>522</x:v>
       </x:c>
     </x:row>
     <x:row r="179" spans="1:6">
       <x:c r="A179" s="1" t="s">
+        <x:v>522</x:v>
+      </x:c>
+      <x:c r="B179" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C179" s="1" t="s">
         <x:v>523</x:v>
       </x:c>
-      <x:c r="B179" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C179" s="1" t="s">
+      <x:c r="F179" s="1" t="s">
         <x:v>524</x:v>
-      </x:c>
-      <x:c r="F179" s="1" t="s">
-        <x:v>525</x:v>
       </x:c>
     </x:row>
     <x:row r="180" spans="1:6">
       <x:c r="A180" s="1" t="s">
+        <x:v>525</x:v>
+      </x:c>
+      <x:c r="B180" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C180" s="1" t="s">
         <x:v>526</x:v>
       </x:c>
-      <x:c r="B180" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C180" s="1" t="s">
+      <x:c r="F180" s="1" t="s">
         <x:v>527</x:v>
-      </x:c>
-      <x:c r="F180" s="1" t="s">
-        <x:v>528</x:v>
       </x:c>
     </x:row>
     <x:row r="181" spans="1:6">
       <x:c r="A181" s="1" t="s">
+        <x:v>528</x:v>
+      </x:c>
+      <x:c r="B181" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C181" s="1" t="s">
         <x:v>529</x:v>
       </x:c>
-      <x:c r="B181" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C181" s="1" t="s">
+      <x:c r="F181" s="1" t="s">
         <x:v>530</x:v>
-      </x:c>
-      <x:c r="F181" s="1" t="s">
-        <x:v>531</x:v>
       </x:c>
     </x:row>
     <x:row r="182" spans="1:6">
       <x:c r="A182" s="1" t="s">
+        <x:v>531</x:v>
+      </x:c>
+      <x:c r="B182" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C182" s="1" t="s">
         <x:v>532</x:v>
       </x:c>
-      <x:c r="B182" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C182" s="1" t="s">
+      <x:c r="F182" s="1" t="s">
         <x:v>533</x:v>
-      </x:c>
-      <x:c r="F182" s="1" t="s">
-        <x:v>534</x:v>
       </x:c>
     </x:row>
     <x:row r="183" spans="1:6">
       <x:c r="A183" s="1" t="s">
+        <x:v>534</x:v>
+      </x:c>
+      <x:c r="B183" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C183" s="1" t="s">
         <x:v>535</x:v>
       </x:c>
-      <x:c r="B183" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C183" s="1" t="s">
+      <x:c r="F183" s="1" t="s">
         <x:v>536</x:v>
-      </x:c>
-      <x:c r="F183" s="1" t="s">
-        <x:v>537</x:v>
       </x:c>
     </x:row>
     <x:row r="184" spans="1:6">
       <x:c r="A184" s="1" t="s">
+        <x:v>537</x:v>
+      </x:c>
+      <x:c r="B184" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C184" s="1" t="s">
         <x:v>538</x:v>
       </x:c>
-      <x:c r="B184" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C184" s="1" t="s">
+      <x:c r="F184" s="1" t="s">
         <x:v>539</x:v>
-      </x:c>
-      <x:c r="F184" s="1" t="s">
-        <x:v>540</x:v>
       </x:c>
     </x:row>
     <x:row r="185" spans="1:6">
       <x:c r="A185" s="1" t="s">
+        <x:v>540</x:v>
+      </x:c>
+      <x:c r="B185" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C185" s="1" t="s">
         <x:v>541</x:v>
       </x:c>
-      <x:c r="B185" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C185" s="1" t="s">
+      <x:c r="F185" s="1" t="s">
         <x:v>542</x:v>
-      </x:c>
-      <x:c r="F185" s="1" t="s">
-        <x:v>543</x:v>
       </x:c>
     </x:row>
     <x:row r="186" spans="1:6">
       <x:c r="A186" s="1" t="s">
+        <x:v>543</x:v>
+      </x:c>
+      <x:c r="B186" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C186" s="1" t="s">
         <x:v>544</x:v>
       </x:c>
-      <x:c r="B186" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C186" s="1" t="s">
+      <x:c r="F186" s="1" t="s">
         <x:v>545</x:v>
-      </x:c>
-      <x:c r="F186" s="1" t="s">
-        <x:v>546</x:v>
       </x:c>
     </x:row>
     <x:row r="187" spans="1:6">
       <x:c r="A187" s="1" t="s">
+        <x:v>546</x:v>
+      </x:c>
+      <x:c r="B187" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C187" s="1" t="s">
         <x:v>547</x:v>
       </x:c>
-      <x:c r="B187" s="1" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="C187" s="1" t="s">
+      <x:c r="F187" s="1" t="s">
         <x:v>548</x:v>
-      </x:c>
-      <x:c r="F187" s="1" t="s">
-        <x:v>285</x:v>
       </x:c>
     </x:row>
     <x:row r="188" spans="1:6">
@@ -4727,7 +4787,7 @@
         <x:v>549</x:v>
       </x:c>
       <x:c r="B188" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C188" s="1" t="s">
         <x:v>550</x:v>
@@ -4741,7 +4801,7 @@
         <x:v>552</x:v>
       </x:c>
       <x:c r="B189" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C189" s="1" t="s">
         <x:v>553</x:v>
@@ -4755,7 +4815,7 @@
         <x:v>555</x:v>
       </x:c>
       <x:c r="B190" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C190" s="1" t="s">
         <x:v>556</x:v>
@@ -4769,7 +4829,7 @@
         <x:v>558</x:v>
       </x:c>
       <x:c r="B191" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C191" s="1" t="s">
         <x:v>559</x:v>
@@ -4783,7 +4843,7 @@
         <x:v>561</x:v>
       </x:c>
       <x:c r="B192" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C192" s="1" t="s">
         <x:v>562</x:v>
@@ -4797,7 +4857,7 @@
         <x:v>564</x:v>
       </x:c>
       <x:c r="B193" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C193" s="1" t="s">
         <x:v>565</x:v>
@@ -4811,13 +4871,111 @@
         <x:v>567</x:v>
       </x:c>
       <x:c r="B194" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="C194" s="1" t="s">
         <x:v>568</x:v>
       </x:c>
       <x:c r="F194" s="1" t="s">
+        <x:v>296</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="195" spans="1:6">
+      <x:c r="A195" s="1" t="s">
         <x:v>569</x:v>
+      </x:c>
+      <x:c r="B195" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C195" s="1" t="s">
+        <x:v>570</x:v>
+      </x:c>
+      <x:c r="F195" s="1" t="s">
+        <x:v>571</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="196" spans="1:6">
+      <x:c r="A196" s="1" t="s">
+        <x:v>572</x:v>
+      </x:c>
+      <x:c r="B196" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C196" s="1" t="s">
+        <x:v>573</x:v>
+      </x:c>
+      <x:c r="F196" s="1" t="s">
+        <x:v>574</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="197" spans="1:6">
+      <x:c r="A197" s="1" t="s">
+        <x:v>575</x:v>
+      </x:c>
+      <x:c r="B197" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C197" s="1" t="s">
+        <x:v>576</x:v>
+      </x:c>
+      <x:c r="F197" s="1" t="s">
+        <x:v>577</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="198" spans="1:6">
+      <x:c r="A198" s="1" t="s">
+        <x:v>578</x:v>
+      </x:c>
+      <x:c r="B198" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C198" s="1" t="s">
+        <x:v>579</x:v>
+      </x:c>
+      <x:c r="F198" s="1" t="s">
+        <x:v>580</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="199" spans="1:6">
+      <x:c r="A199" s="1" t="s">
+        <x:v>581</x:v>
+      </x:c>
+      <x:c r="B199" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C199" s="1" t="s">
+        <x:v>582</x:v>
+      </x:c>
+      <x:c r="F199" s="1" t="s">
+        <x:v>583</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="200" spans="1:6">
+      <x:c r="A200" s="1" t="s">
+        <x:v>584</x:v>
+      </x:c>
+      <x:c r="B200" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C200" s="1" t="s">
+        <x:v>585</x:v>
+      </x:c>
+      <x:c r="F200" s="1" t="s">
+        <x:v>586</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="201" spans="1:6">
+      <x:c r="A201" s="1" t="s">
+        <x:v>587</x:v>
+      </x:c>
+      <x:c r="B201" s="1" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="C201" s="1" t="s">
+        <x:v>588</x:v>
+      </x:c>
+      <x:c r="F201" s="1" t="s">
+        <x:v>589</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>